<commit_message>
Update Mobil alkalmazásfejlesztés projektmunka pontozás.xlsx
</commit_message>
<xml_diff>
--- a/Mobil alkalmazásfejlesztés projektmunka pontozás.xlsx
+++ b/Mobil alkalmazásfejlesztés projektmunka pontozás.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prog_gyors\project assets\Mobil_alk_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B1FD7D-2D4B-40E9-BAEC-D84AA937A813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260D9A36-A52E-4096-A0B4-704B17641703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -647,14 +647,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:4" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="19">
         <v>2</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="20" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>